<commit_message>
adding realtime and prediction function
</commit_message>
<xml_diff>
--- a/svm_br/results/observations.xlsx
+++ b/svm_br/results/observations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>exper.no.</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>TTP+TNA+angels between fingers</t>
+  </si>
+  <si>
+    <t>The best parameters are {'C': 10.0, 'gamma': 1e-09} with a score of 0.98</t>
+  </si>
+  <si>
+    <t>linear</t>
   </si>
 </sst>
 </file>
@@ -164,7 +170,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,6 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -461,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,6 +848,80 @@
         <v>28</v>
       </c>
     </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="E37" s="8">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37">
+        <v>0.90419161676646698</v>
+      </c>
+      <c r="K37" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>1000</v>
+      </c>
+      <c r="E38">
+        <v>0.01</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38">
+        <v>0.90269461077844304</v>
+      </c>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>1000000</v>
+      </c>
+      <c r="E39">
+        <v>0.01</v>
+      </c>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39">
+        <v>0.90269461077844304</v>
+      </c>
+      <c r="K39" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>